<commit_message>
premint chain stuck fix
</commit_message>
<xml_diff>
--- a/files/wallet.xlsx
+++ b/files/wallet.xlsx
@@ -25,7 +25,7 @@
     <t>Private Key</t>
   </si>
   <si>
-    <t>g</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -101,16 +101,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -423,9 +426,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -444,7 +447,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
+      <c r="C2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>